<commit_message>
Added more characters/categories. Work on document: some drawings, graphics, and added comparison on simplification methods.
</commit_message>
<xml_diff>
--- a/data/quality_results.xlsx
+++ b/data/quality_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="3120" windowWidth="7125" windowHeight="1875"/>
+    <workbookView xWindow="3435" yWindow="3120" windowWidth="7125" windowHeight="1875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw data" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -435,6 +435,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -444,18 +453,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BZ52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="X44" sqref="X44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,38 +1079,38 @@
       <c r="B5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="19" t="s">
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="19" t="s">
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="21"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="30"/>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
@@ -1128,11 +1131,11 @@
       <c r="AT5" s="11"/>
       <c r="AU5" s="11"/>
       <c r="AV5" s="11"/>
-      <c r="AW5" s="20" t="s">
+      <c r="AW5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="AX5" s="20"/>
-      <c r="AY5" s="21"/>
+      <c r="AX5" s="29"/>
+      <c r="AY5" s="30"/>
       <c r="AZ5" s="2"/>
       <c r="BA5" s="2"/>
       <c r="BB5" s="2"/>
@@ -3518,38 +3521,38 @@
       <c r="B19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="19" t="s">
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20"/>
-      <c r="Z19" s="20" t="s">
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="21"/>
+      <c r="AA19" s="29"/>
+      <c r="AB19" s="30"/>
       <c r="AC19" s="11"/>
       <c r="AD19" s="11"/>
       <c r="AE19" s="11"/>
@@ -3570,11 +3573,11 @@
       <c r="AT19" s="11"/>
       <c r="AU19" s="11"/>
       <c r="AV19" s="11"/>
-      <c r="AW19" s="20" t="s">
+      <c r="AW19" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="AX19" s="20"/>
-      <c r="AY19" s="21"/>
+      <c r="AX19" s="29"/>
+      <c r="AY19" s="30"/>
       <c r="AZ19" s="2"/>
       <c r="BA19" s="2"/>
       <c r="BB19" s="2"/>
@@ -5857,38 +5860,38 @@
       <c r="B33" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
-      <c r="U33" s="20"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="19" t="s">
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
+      <c r="T33" s="29"/>
+      <c r="U33" s="29"/>
+      <c r="V33" s="30"/>
+      <c r="W33" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="X33" s="20"/>
-      <c r="Y33" s="21"/>
-      <c r="Z33" s="19" t="s">
+      <c r="X33" s="29"/>
+      <c r="Y33" s="30"/>
+      <c r="Z33" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AA33" s="20"/>
-      <c r="AB33" s="21"/>
+      <c r="AA33" s="29"/>
+      <c r="AB33" s="30"/>
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
       <c r="AE33" s="2"/>
@@ -5909,11 +5912,11 @@
       <c r="AT33" s="2"/>
       <c r="AU33" s="2"/>
       <c r="AV33" s="2"/>
-      <c r="AW33" s="19" t="s">
+      <c r="AW33" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="AX33" s="20"/>
-      <c r="AY33" s="21"/>
+      <c r="AX33" s="29"/>
+      <c r="AY33" s="30"/>
     </row>
     <row r="34" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
@@ -8363,163 +8366,167 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="31" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="31" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="27"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="25" t="s">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="23" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="24">
+      <c r="A4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="31">
         <v>0.84444444444444444</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="32">
         <v>0.76666666666666661</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="33">
         <v>0.75555555555555565</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="31">
         <v>0.73333333333333328</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="32">
         <v>0.56666666666666665</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="33">
         <v>0.4555555555555556</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="31">
         <v>6.9890740457885174</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="32">
         <v>9.392224444125981</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="33">
         <v>12.066306168648717</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="31">
         <v>0.88888888888888884</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="32">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="33">
         <v>0.74444444444444446</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="31">
         <v>0.82222222222222219</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="32">
         <v>0.66666666666666663</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="33">
         <v>0.51666666666666672</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="31">
         <v>7.473270152778456</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="32">
         <v>10.383854372092836</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="33">
         <v>13.868233715443559</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="34">
         <v>0.91111111111111098</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="35">
         <v>0.93333333333333335</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="36">
         <v>0.87222222222222223</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="34">
         <v>0.82222222222222219</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="35">
         <v>0.81111111111111112</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="36">
         <v>0.6166666666666667</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="34">
         <v>7.5296230007047518</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="35">
         <v>11.614769661890849</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="36">
         <v>15.797467638460009</v>
       </c>
     </row>

</xml_diff>